<commit_message>
fhir ig initial setup
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ethnic-code.xlsx
+++ b/output/StructureDefinition-ethnic-code.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-19T07:52:08+05:45</t>
+    <t>2025-08-20T08:30:34+05:45</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -135,7 +135,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Element</t>
+    <t>element:Patient</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>